<commit_message>
reestructuracion y limpieza del codigo. Adicion de documentacion para los programadores en Sound Lab Programing Guide
</commit_message>
<xml_diff>
--- a/Sound Lab Programing Guide/DUETTO SOUND LAB ISSUES .xlsx
+++ b/Sound Lab Programing Guide/DUETTO SOUND LAB ISSUES .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -411,7 +411,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,9 @@
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>